<commit_message>
Updated Requirements after review by Marten Wensink
</commit_message>
<xml_diff>
--- a/Analyse en ontwerp/Requirements Analyse/RequirementsLaserQuest.xlsx
+++ b/Analyse en ontwerp/Requirements Analyse/RequirementsLaserQuest.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17520"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hogeschoolutrecht.sharepoint.com/sites/tekteamone/Gedeelde  documenten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Arco/Documents/TekTeamOne/Analyse en ontwerp/Requirements Analyse/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="7_{A655D982-98FC-4586-9121-1BA86D319FC6}" xr6:coauthVersionLast="10" xr6:coauthVersionMax="10" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33600" yWindow="-9795" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16760" windowHeight="21000"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171026" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="43">
   <si>
     <t>Requirements (zo specifiek mogelijk)</t>
   </si>
@@ -66,9 +65,6 @@
     <t>Het is mogelijk de gegevens die op de Arduino staan aangaande het spel uit te lezen op een computer door middel van een USB verbinding</t>
   </si>
   <si>
-    <t>Er kan een wapen gekozen worden op basis van schade per kogel</t>
-  </si>
-  <si>
     <t>Audiosignaal van 3 seconden op 1000Hz bij start</t>
   </si>
   <si>
@@ -154,13 +150,19 @@
   </si>
   <si>
     <t>Camera die checkt of er echt op jou geschoten is, niet dat het slechts wat diffuus licht is</t>
+  </si>
+  <si>
+    <t>Er kan een wapen gekozen worden op basis van schade per kogel (waarden tussen 0 en 100)</t>
+  </si>
+  <si>
+    <t>Counter die de speltijd bijhoudt en vergelijkt met de eerder ingestelde totale speltijd, wanneer deze gelijk zijn betekend dit het einde van het spel</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -338,7 +340,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -649,22 +651,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E38"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10:B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="92.42578125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.42578125" customWidth="1"/>
+    <col min="1" max="1" width="92.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="5" max="5" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="21">
+    <row r="1" spans="1:2" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -672,7 +674,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="12" t="s">
         <v>2</v>
       </c>
@@ -680,7 +682,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
@@ -688,7 +690,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
@@ -696,7 +698,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -704,7 +706,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -712,7 +714,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -720,7 +722,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>9</v>
       </c>
@@ -728,7 +730,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>10</v>
       </c>
@@ -736,236 +738,244 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="30">
+    <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
-      <c r="A11" s="3" t="s">
+      <c r="B11" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
-      <c r="A12" s="3" t="s">
+      <c r="B13" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B12" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
-      <c r="A13" s="3" t="s">
+      <c r="B14" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
-      <c r="A14" s="3" t="s">
+      <c r="B15" s="6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B14" s="6" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
-      <c r="A15" s="4" t="s">
+      <c r="B16" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B15" s="7" t="s">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:2">
-      <c r="A16" s="4" t="s">
+      <c r="B17" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B16" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" ht="30">
-      <c r="A17" s="4" t="s">
+      <c r="B18" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B17" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" ht="30">
-      <c r="A18" s="4" t="s">
+      <c r="B19" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="A19" s="4" t="s">
+      <c r="B20" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A21" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B19" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="30">
-      <c r="A20" s="4" t="s">
+      <c r="B21" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B20" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="A21" s="4" t="s">
+      <c r="B22" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="B21" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15" customHeight="1">
-      <c r="A22" s="4" t="s">
+      <c r="B23" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A24" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="7" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="30">
-      <c r="A23" s="13" t="s">
+      <c r="B24" s="16" t="s">
         <v>25</v>
       </c>
-      <c r="B23" s="16" t="s">
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A25" s="15" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="30">
-      <c r="A24" s="15" t="s">
+      <c r="B25" s="17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="B24" s="17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:5">
-      <c r="A25" s="13" t="s">
+      <c r="B26" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="B25" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5">
-      <c r="A26" s="13" t="s">
+      <c r="B27" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="B26" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5">
-      <c r="A27" s="13" t="s">
+      <c r="B28" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A29" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" ht="30">
-      <c r="A28" s="13" t="s">
+      <c r="B29" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="B28" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E28" s="2"/>
-    </row>
-    <row r="29" spans="1:5" ht="14.25" customHeight="1">
-      <c r="A29" s="13" t="s">
+      <c r="B30" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E30" s="2"/>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E29" s="2"/>
-    </row>
-    <row r="30" spans="1:5">
-      <c r="A30" s="13" t="s">
+      <c r="B31" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="B30" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E30" s="2"/>
-    </row>
-    <row r="31" spans="1:5">
-      <c r="A31" s="13" t="s">
+      <c r="B32" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="B31" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E31" s="2"/>
-    </row>
-    <row r="32" spans="1:5" ht="15.75" customHeight="1">
-      <c r="A32" s="13" t="s">
+      <c r="B33" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A34" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="B32" s="14" t="s">
-        <v>26</v>
-      </c>
-      <c r="E32" s="2"/>
-    </row>
-    <row r="33" spans="1:2" ht="30">
-      <c r="A33" s="13" t="s">
+      <c r="B34" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="B33" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
-      <c r="A34" s="13" t="s">
+      <c r="B35" s="14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="B34" s="14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
-      <c r="A35" s="5" t="s">
+      <c r="B36" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B35" s="8" t="s">
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="5" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="5" t="s">
+      <c r="B37" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="B36" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
-      <c r="A37" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" ht="15.75" customHeight="1"/>
+      <c r="B38" s="8" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <sortState ref="A2:C37">
     <sortCondition ref="B2:B37"/>
@@ -975,21 +985,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005482E0FAFE580A4A90AE260043697E6F" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8fb62b114feff957bfd4cb8ec2a11fe0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="15ce71b8-92b5-4d42-93e0-fad89e64317b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6c03c8688e14a8719cdd4030430179e" ns2:_="">
     <xsd:import namespace="15ce71b8-92b5-4d42-93e0-fad89e64317b"/>
@@ -1137,31 +1132,22 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EC03CBD-7640-4B3A-A280-C89DCC8C2C0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A29786DB-CC1C-466B-8A97-6FABF74EB7EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="15ce71b8-92b5-4d42-93e0-fad89e64317b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C87AFCF-834D-46B5-A653-60999E12454B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1177,4 +1163,28 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EC03CBD-7640-4B3A-A280-C89DCC8C2C0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A29786DB-CC1C-466B-8A97-6FABF74EB7EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="15ce71b8-92b5-4d42-93e0-fad89e64317b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Fully update requirements analyse
</commit_message>
<xml_diff>
--- a/Analyse en ontwerp/Requirements Analyse/RequirementsLaserQuest.xlsx
+++ b/Analyse en ontwerp/Requirements Analyse/RequirementsLaserQuest.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Arco/Documents/TekTeamOne/Analyse en ontwerp/Requirements Analyse/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Arco/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16760" windowHeight="21000"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="33600" windowHeight="19740"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -71,9 +71,6 @@
     <t>Audiosignaal van 3 seconden op 1000Hz bij einde</t>
   </si>
   <si>
-    <t>Foutmeldingen worden gemeld aan de gebruiker en aan de admin</t>
-  </si>
-  <si>
     <t>De registratie van het aantal schoten (Gebeurt bij de schietende speler)</t>
   </si>
   <si>
@@ -134,9 +131,6 @@
     <t>Er brand een LED om te specificren in welk team de speler zit, het verschil zal te zien zijn door de kleur van de LED</t>
   </si>
   <si>
-    <t>Wanneer een speler geen hitpoints meer heeft (en dus 'dood' is) wordt dit bekend gemaakt door een piepend geluidssignaal voor 3 seconden</t>
-  </si>
-  <si>
     <t>Specifiek ledje knippert 10 seconden bij nul HP om te specificeren dat je 10 seconden niet mag schieten.</t>
   </si>
   <si>
@@ -150,6 +144,12 @@
   </si>
   <si>
     <t>Camera die checkt of er echt op jou geschoten is, niet dat het slechts wat diffuus licht is</t>
+  </si>
+  <si>
+    <t>Foutmelding wordt weergegeven op de lasergun door middel van LED</t>
+  </si>
+  <si>
+    <t>Wanneer een speler geen hitpoints meer heeft (en dus 'dood' is) wordt dit bekend gemaakt door een geluidssignaal van 1000Hz en kan de speler het wapen 3 seconden niet gebruiken</t>
   </si>
   <si>
     <t>Er kan een wapen gekozen worden op basis van schade per kogel (waarden tussen 0 en 100)</t>
@@ -656,13 +656,14 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A10" sqref="A10:B10"/>
+      <selection pane="bottomLeft" activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="92.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.83203125" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -740,7 +741,7 @@
     </row>
     <row r="10" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>42</v>
+        <v>11</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>3</v>
@@ -748,7 +749,7 @@
     </row>
     <row r="11" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>11</v>
+        <v>42</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>3</v>
@@ -780,7 +781,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>3</v>
@@ -788,191 +789,191 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B16" s="7" t="s">
         <v>15</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>24</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B26" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B27" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B28" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B29" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E29" s="2"/>
     </row>
     <row r="30" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B30" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E30" s="2"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="13" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B31" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E31" s="2"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B32" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E32" s="2"/>
     </row>
     <row r="33" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="13" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B33" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="E33" s="2"/>
     </row>
     <row r="34" spans="1:5" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B34" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B35" s="14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="5" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B37" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B38" s="8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -985,6 +986,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005482E0FAFE580A4A90AE260043697E6F" ma:contentTypeVersion="2" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="8fb62b114feff957bfd4cb8ec2a11fe0">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="15ce71b8-92b5-4d42-93e0-fad89e64317b" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a6c03c8688e14a8719cdd4030430179e" ns2:_="">
     <xsd:import namespace="15ce71b8-92b5-4d42-93e0-fad89e64317b"/>
@@ -1132,22 +1148,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EC03CBD-7640-4B3A-A280-C89DCC8C2C0D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A29786DB-CC1C-466B-8A97-6FABF74EB7EE}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="15ce71b8-92b5-4d42-93e0-fad89e64317b"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3C87AFCF-834D-46B5-A653-60999E12454B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1163,28 +1188,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8EC03CBD-7640-4B3A-A280-C89DCC8C2C0D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A29786DB-CC1C-466B-8A97-6FABF74EB7EE}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="15ce71b8-92b5-4d42-93e0-fad89e64317b"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>